<commit_message>
Updated html, css and js
</commit_message>
<xml_diff>
--- a/Wine-Food Tables.xlsx
+++ b/Wine-Food Tables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d5f8bb61184e319/Desktop/Documents/Coding Bootcamp/project2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arifa\OneDrive\Desktop\Documents\Coding Bootcamp\project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F290A9E-A0F2-4123-A901-B0A67191305B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="8_{0F290A9E-A0F2-4123-A901-B0A67191305B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{A5C22853-DA12-47EB-A386-DC1EF96DBEE9}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{B6F93CE3-C963-4B74-BB5E-CEF4A19E555E}"/>
   </bookViews>
@@ -24,15 +24,306 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+  <si>
+    <t>Malbec</t>
+  </si>
+  <si>
+    <t>Syrah/Shiraz</t>
+  </si>
+  <si>
+    <t>Cabarnet Sauvignon</t>
+  </si>
+  <si>
+    <t>Bordeaux Blend</t>
+  </si>
+  <si>
+    <t>Merlot</t>
+  </si>
+  <si>
+    <t>Zinfandel</t>
+  </si>
+  <si>
+    <t>Pinot Noir</t>
+  </si>
+  <si>
+    <t>Gamay</t>
+  </si>
+  <si>
+    <t>All Roses</t>
+  </si>
+  <si>
+    <t>Sauvignon Blanc</t>
+  </si>
+  <si>
+    <t>Pinot Blanc</t>
+  </si>
+  <si>
+    <t>Pinot Gris</t>
+  </si>
+  <si>
+    <t>Champagne</t>
+  </si>
+  <si>
+    <t>Prosecco</t>
+  </si>
+  <si>
+    <t>Sparkling Rose</t>
+  </si>
+  <si>
+    <t>Moscato</t>
+  </si>
+  <si>
+    <t>Riesling</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>Sherry</t>
+  </si>
+  <si>
+    <t>Madeira</t>
+  </si>
+  <si>
+    <t>Muscat</t>
+  </si>
+  <si>
+    <t>"RED"&gt;</t>
+  </si>
+  <si>
+    <t>"ROSE"&gt;</t>
+  </si>
+  <si>
+    <t>LIGHT WHITE"&gt;</t>
+  </si>
+  <si>
+    <t>"SPARKLING"&gt;</t>
+  </si>
+  <si>
+    <t>"SWEET WHITE/DESSERT"&gt;</t>
+  </si>
+  <si>
+    <t>Wine Table</t>
+  </si>
+  <si>
+    <t>Food Table</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"MEAT"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Red Meat(beef/lamb)</t>
+  </si>
+  <si>
+    <t>Cured Meat(bacon/salami)</t>
+  </si>
+  <si>
+    <t>Pork(roast/tenderloin/chop)</t>
+  </si>
+  <si>
+    <t>Poultry(chicken/duck/turkey)</t>
+  </si>
+  <si>
+    <t>Mollusk(oyster/mussel/clam)</t>
+  </si>
+  <si>
+    <t>Fish(tuna/cod/trout/bass)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"DAIRY"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Soft Cheese</t>
+  </si>
+  <si>
+    <t>Hard Cheese</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"VEGETABLE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Green Vegetables(lettuce/kale)</t>
+  </si>
+  <si>
+    <t>Root Vegetables(pumpkin/carrot)</t>
+  </si>
+  <si>
+    <t>Nightshades(tomato/eggplant)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"SWEET"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Lobster &amp; Shellfish(prawn/crab)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Nuts &amp; Seeds</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Fruit &amp; Berries(strawberry/orange/apple)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Vanilla &amp; Caramel(creme brulee/ice cream)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Chocolate &amp; Coffee</t>
+    </r>
+  </si>
+  <si>
+    <t>Chardonnay</t>
+  </si>
+  <si>
+    <t>FK2(wine)</t>
+  </si>
+  <si>
+    <t>FK1(food)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF808080"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -55,8 +346,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,12 +669,521 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5104259-2E91-49ED-B0BC-77D4299EC1DC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="48.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="1"/>
+      <c r="E20">
+        <v>8</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>8</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>7</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>9</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="1"/>
+      <c r="E25">
+        <v>9</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>8</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>8</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>9</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>9</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>9</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>